<commit_message>
atualizando ciclo de vida
</commit_message>
<xml_diff>
--- a/17. Análise dos Eventos Para Cada Cenário.xlsx
+++ b/17. Análise dos Eventos Para Cada Cenário.xlsx
@@ -864,6 +864,48 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -881,48 +923,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,25 +1244,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="41"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="47" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="47" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="48"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="62"/>
       <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="17.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1289,10 +1289,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="66" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6">
@@ -1311,8 +1311,8 @@
       <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="53"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1329,8 +1329,8 @@
       <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="53"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="7">
         <v>3</v>
       </c>
@@ -1347,8 +1347,8 @@
       <c r="J5" s="44"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="53"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="8">
         <v>4</v>
       </c>
@@ -1365,10 +1365,10 @@
       <c r="J6" s="44"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3">
@@ -1387,8 +1387,8 @@
       <c r="J7" s="44"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="55"/>
-      <c r="B8" s="66"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="3">
         <v>6</v>
       </c>
@@ -1405,8 +1405,8 @@
       <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="55"/>
-      <c r="B9" s="66"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="3">
         <v>7</v>
       </c>
@@ -1423,8 +1423,8 @@
       <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="55"/>
-      <c r="B10" s="66"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="9">
         <v>8</v>
       </c>
@@ -1441,8 +1441,8 @@
       <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="55"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="16">
         <v>9</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A12" s="55"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="36" t="s">
         <v>36</v>
       </c>
@@ -1479,10 +1479,10 @@
       <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8">
@@ -1501,8 +1501,8 @@
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1">
-      <c r="A14" s="57"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="8">
         <v>12</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="51" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -1563,7 +1563,7 @@
       <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A17" s="59"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
@@ -1584,17 +1584,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B7:B11"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>